<commit_message>
FINALLY DOING SOME WORK
</commit_message>
<xml_diff>
--- a/20Questions.xlsx
+++ b/20Questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/20arjuna/Desktop/Jess71p1/ExpertSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930A1DC7-D41E-4D4E-A1AC-28A62147B99F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099D157C-04D3-9E4E-88B6-85A0318C22AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16000" xr2:uid="{84C34A19-7255-F447-B18A-1F0426312428}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="16000" xr2:uid="{84C34A19-7255-F447-B18A-1F0426312428}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="85">
   <si>
     <t>is it a mammal</t>
   </si>
@@ -208,6 +208,84 @@
   </si>
   <si>
     <t>panda?</t>
+  </si>
+  <si>
+    <t>panda</t>
+  </si>
+  <si>
+    <t>Adrian #4</t>
+  </si>
+  <si>
+    <t>mammal</t>
+  </si>
+  <si>
+    <t>on land</t>
+  </si>
+  <si>
+    <t>ominvor</t>
+  </si>
+  <si>
+    <t>carnivore</t>
+  </si>
+  <si>
+    <t>African</t>
+  </si>
+  <si>
+    <t>long neck</t>
+  </si>
+  <si>
+    <t>giraffe</t>
+  </si>
+  <si>
+    <t>Giraffe</t>
+  </si>
+  <si>
+    <t>Adrian #5</t>
+  </si>
+  <si>
+    <t>on land?</t>
+  </si>
+  <si>
+    <t>sometimes</t>
+  </si>
+  <si>
+    <t>2 legs</t>
+  </si>
+  <si>
+    <t>reptile</t>
+  </si>
+  <si>
+    <t>crab?</t>
+  </si>
+  <si>
+    <t>vertibrate?</t>
+  </si>
+  <si>
+    <t>live on beach?</t>
+  </si>
+  <si>
+    <t>near water?</t>
+  </si>
+  <si>
+    <t>near river?</t>
+  </si>
+  <si>
+    <t>near lake?</t>
+  </si>
+  <si>
+    <t>cold temperatures?</t>
+  </si>
+  <si>
+    <t>dangerous?</t>
+  </si>
+  <si>
+    <t>zoo?</t>
+  </si>
+  <si>
+    <t>swim</t>
+  </si>
+  <si>
+    <t>penguin</t>
   </si>
 </sst>
 </file>
@@ -562,15 +640,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759C4F4A-D4BB-9940-B286-32E03A09D8CF}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -580,8 +658,14 @@
       <c r="J1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,8 +684,20 @@
       <c r="L2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -620,8 +716,20 @@
       <c r="L3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>70</v>
+      </c>
+      <c r="U3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -640,8 +748,20 @@
       <c r="L4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -660,8 +780,20 @@
       <c r="L5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -680,8 +812,20 @@
       <c r="L6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -700,8 +844,20 @@
       <c r="L7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -720,8 +876,20 @@
       <c r="L8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>74</v>
+      </c>
+      <c r="U8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -740,8 +908,20 @@
       <c r="L9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>75</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -760,8 +940,20 @@
       <c r="L10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -780,8 +972,14 @@
       <c r="L11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>77</v>
+      </c>
+      <c r="U11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -800,8 +998,14 @@
       <c r="L12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S12" t="s">
+        <v>78</v>
+      </c>
+      <c r="U12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -820,8 +1024,14 @@
       <c r="L13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>79</v>
+      </c>
+      <c r="U13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -840,8 +1050,14 @@
       <c r="L14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S14" t="s">
+        <v>80</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -854,8 +1070,14 @@
       <c r="L15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S15" t="s">
+        <v>81</v>
+      </c>
+      <c r="U15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -868,8 +1090,14 @@
       <c r="L16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S16" t="s">
+        <v>82</v>
+      </c>
+      <c r="U16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -882,8 +1110,14 @@
       <c r="L17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="S17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -897,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -911,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -919,12 +1153,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="F22" t="s">
         <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>59</v>
+      </c>
+      <c r="O22" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>